<commit_message>
Get ugly timeline up
</commit_message>
<xml_diff>
--- a/web/d3/data/work-dates.xlsx
+++ b/web/d3/data/work-dates.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="75">
   <si>
     <t xml:space="preserve">WorkTitle</t>
   </si>
@@ -256,9 +256,6 @@
   </si>
   <si>
     <t xml:space="preserve">correcting proofs of part I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">война и мир </t>
   </si>
   <si>
     <t xml:space="preserve">Part II</t>
@@ -424,19 +421,21 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="A:I"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.0925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.6296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.9666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.462962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.5111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.1111111111111"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1349,7 +1348,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>68</v>
@@ -1358,7 +1357,7 @@
         <v>11</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F38" s="4" t="n">
         <v>-12722</v>
@@ -1383,7 +1382,7 @@
         <v>11</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F39" s="4" t="n">
         <v>-12477</v>
@@ -1408,7 +1407,7 @@
         <v>11</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F40" s="4" t="n">
         <v>-12402</v>

</xml_diff>